<commit_message>
Update of bill of material to reflect 4_14_16 build
</commit_message>
<xml_diff>
--- a/Eurocard-HV-piezo-driver_default_BOM_values.xlsx
+++ b/Eurocard-HV-piezo-driver_default_BOM_values.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="21075" windowHeight="11310"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="21075" windowHeight="10050"/>
   </bookViews>
   <sheets>
     <sheet name="Eurocard-HV-piezo-driver_defaul" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="250">
   <si>
     <t>Qty</t>
   </si>
@@ -697,9 +697,6 @@
     <t xml:space="preserve">RR08P20.5KDCT-ND </t>
   </si>
   <si>
-    <t>R2, R26,R32</t>
-  </si>
-  <si>
     <t>445-14276-1-ND</t>
   </si>
   <si>
@@ -755,13 +752,25 @@
   </si>
   <si>
     <t>Quantity Available (after additional Digikey purchase)</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>diodes need reference indicator in package!!!!!!! U6,U7 as well</t>
+  </si>
+  <si>
+    <t>R2,R32</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -901,6 +910,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1307,7 +1324,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1338,10 +1355,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1687,8 +1705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M56" sqref="M56"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1706,19 +1724,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>245</v>
+      <c r="A1" s="19" t="s">
+        <v>244</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
+      <c r="A2" s="19"/>
       <c r="B2" s="3"/>
       <c r="C2" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1762,13 +1788,16 @@
         <v>12</v>
       </c>
       <c r="O6" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P6" s="17" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>246</v>
+      </c>
       <c r="B7" s="8">
         <v>20</v>
       </c>
@@ -1794,14 +1823,17 @@
         <v>55</v>
       </c>
       <c r="O7">
-        <v>580</v>
-      </c>
-      <c r="P7" s="19">
+        <v>560</v>
+      </c>
+      <c r="P7" s="18">
         <f>FLOOR(O7/B7,1)</f>
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>246</v>
+      </c>
       <c r="B8" s="3">
         <v>1</v>
       </c>
@@ -1827,14 +1859,17 @@
         <v>65</v>
       </c>
       <c r="O8">
-        <v>29</v>
-      </c>
-      <c r="P8" s="19">
-        <f t="shared" ref="P8:P71" si="0">FLOOR(O8/B8,1)</f>
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="P8" s="18">
+        <f t="shared" ref="P8:P69" si="0">FLOOR(O8/B8,1)</f>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>246</v>
+      </c>
       <c r="B9" s="3">
         <v>4</v>
       </c>
@@ -1860,14 +1895,17 @@
         <v>69</v>
       </c>
       <c r="O9">
-        <v>116</v>
-      </c>
-      <c r="P9" s="19">
-        <f t="shared" si="0"/>
-        <v>29</v>
+        <v>112</v>
+      </c>
+      <c r="P9" s="18">
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>246</v>
+      </c>
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1893,14 +1931,17 @@
         <v>73</v>
       </c>
       <c r="O10">
-        <v>29</v>
-      </c>
-      <c r="P10" s="19">
-        <f t="shared" si="0"/>
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="P10" s="18">
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>246</v>
+      </c>
       <c r="B11" s="6">
         <v>1</v>
       </c>
@@ -1921,17 +1962,20 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O11">
-        <v>100</v>
-      </c>
-      <c r="P11" s="19">
-        <f t="shared" si="0"/>
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="P11" s="18">
+        <f t="shared" si="0"/>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>246</v>
+      </c>
       <c r="B12" s="3">
         <v>27</v>
       </c>
@@ -1958,15 +2002,18 @@
       </c>
       <c r="N12" s="3"/>
       <c r="O12" s="5">
-        <f>1000-27</f>
-        <v>973</v>
-      </c>
-      <c r="P12" s="19">
-        <f t="shared" si="0"/>
-        <v>36</v>
+        <f>973-27</f>
+        <v>946</v>
+      </c>
+      <c r="P12" s="18">
+        <f t="shared" si="0"/>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>246</v>
+      </c>
       <c r="B13" s="6">
         <v>1</v>
       </c>
@@ -1989,17 +2036,20 @@
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O13">
-        <v>100</v>
-      </c>
-      <c r="P13" s="19">
-        <f t="shared" si="0"/>
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="P13" s="18">
+        <f t="shared" si="0"/>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>246</v>
+      </c>
       <c r="B14" s="3">
         <v>2</v>
       </c>
@@ -2026,15 +2076,17 @@
       </c>
       <c r="N14" s="3"/>
       <c r="O14" s="5">
-        <f>29+60</f>
-        <v>89</v>
-      </c>
-      <c r="P14" s="19">
-        <f t="shared" si="0"/>
-        <v>44</v>
+        <v>87</v>
+      </c>
+      <c r="P14" s="18">
+        <f t="shared" si="0"/>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>246</v>
+      </c>
       <c r="B15" s="6">
         <v>3</v>
       </c>
@@ -2045,7 +2097,7 @@
         <v>56</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>41</v>
@@ -2060,11 +2112,11 @@
         <v>58</v>
       </c>
       <c r="O15">
-        <v>100</v>
-      </c>
-      <c r="P15" s="19">
-        <f t="shared" si="0"/>
-        <v>33</v>
+        <v>97</v>
+      </c>
+      <c r="P15" s="18">
+        <f t="shared" si="0"/>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -2090,12 +2142,15 @@
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
       <c r="M16" s="14"/>
-      <c r="P16" s="19">
+      <c r="P16" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>246</v>
+      </c>
       <c r="B17" s="6">
         <v>1</v>
       </c>
@@ -2118,20 +2173,23 @@
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="O17">
-        <v>100</v>
-      </c>
-      <c r="P17" s="19">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="P18" s="19"/>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="P17" s="18">
+        <f t="shared" si="0"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P18" s="18"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>246</v>
+      </c>
       <c r="B19" s="3">
         <v>4</v>
       </c>
@@ -2142,7 +2200,7 @@
         <v>56</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>41</v>
@@ -2158,17 +2216,20 @@
       </c>
       <c r="N19" s="3"/>
       <c r="O19" s="5">
-        <v>98</v>
-      </c>
-      <c r="P19" s="19">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="P20" s="19"/>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="P19" s="18">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P20" s="18"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>246</v>
+      </c>
       <c r="B21" s="8">
         <v>1</v>
       </c>
@@ -2194,14 +2255,17 @@
         <v>49</v>
       </c>
       <c r="O21">
-        <v>29</v>
-      </c>
-      <c r="P21" s="19">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="P21" s="18">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>246</v>
+      </c>
       <c r="B22" s="3">
         <v>1</v>
       </c>
@@ -2229,14 +2293,17 @@
         <v>88</v>
       </c>
       <c r="O22">
-        <v>29</v>
-      </c>
-      <c r="P22" s="19">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="P22" s="18">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>246</v>
+      </c>
       <c r="B23" s="3">
         <v>1</v>
       </c>
@@ -2262,14 +2329,17 @@
         <v>215</v>
       </c>
       <c r="O23">
-        <v>27</v>
-      </c>
-      <c r="P23" s="19">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="P23" s="18">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>246</v>
+      </c>
       <c r="B24" s="3">
         <v>5</v>
       </c>
@@ -2297,14 +2367,17 @@
         <v>83</v>
       </c>
       <c r="O24">
-        <v>145</v>
-      </c>
-      <c r="P24" s="19">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="P24" s="18">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>246</v>
+      </c>
       <c r="B25" s="3">
         <v>1</v>
       </c>
@@ -2330,14 +2403,14 @@
         <v>26</v>
       </c>
       <c r="O25">
-        <v>27</v>
-      </c>
-      <c r="P25" s="19">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="P25" s="18">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <v>2</v>
       </c>
@@ -2365,12 +2438,12 @@
       <c r="O26">
         <v>50</v>
       </c>
-      <c r="P26" s="19">
+      <c r="P26" s="18">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>3</v>
       </c>
@@ -2395,20 +2468,23 @@
       <c r="M27" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="P27" s="19">
+      <c r="P27" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>246</v>
+      </c>
       <c r="B28" s="6">
         <v>1</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>111</v>
@@ -2431,17 +2507,20 @@
         <v>115</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O28">
         <v>29</v>
       </c>
-      <c r="P28" s="19">
+      <c r="P28" s="18">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>246</v>
+      </c>
       <c r="B29" s="3">
         <v>1</v>
       </c>
@@ -2471,12 +2550,12 @@
       <c r="O29">
         <v>29</v>
       </c>
-      <c r="P29" s="19">
+      <c r="P29" s="18">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>1</v>
       </c>
@@ -2495,12 +2574,12 @@
       <c r="M30" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="P30" s="19">
+      <c r="P30" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B31" s="6">
         <v>2</v>
       </c>
@@ -2530,12 +2609,12 @@
       <c r="O31">
         <v>100</v>
       </c>
-      <c r="P31" s="19">
+      <c r="P31" s="18">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B32" s="6">
         <v>1</v>
       </c>
@@ -2565,12 +2644,12 @@
       <c r="O32">
         <v>50</v>
       </c>
-      <c r="P32" s="19">
+      <c r="P32" s="18">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B33" s="6">
         <v>1</v>
       </c>
@@ -2598,12 +2677,12 @@
       <c r="O33">
         <v>29</v>
       </c>
-      <c r="P33" s="19">
+      <c r="P33" s="18">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
         <v>1</v>
       </c>
@@ -2622,12 +2701,12 @@
       <c r="M34" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="P34" s="19">
+      <c r="P34" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
         <v>1</v>
       </c>
@@ -2646,12 +2725,15 @@
       <c r="G35" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="P35" s="19">
+      <c r="P35" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>246</v>
+      </c>
       <c r="B36" s="3">
         <v>10</v>
       </c>
@@ -2677,17 +2759,20 @@
         <v>104</v>
       </c>
       <c r="O36">
-        <v>290</v>
-      </c>
-      <c r="P36" s="19">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="P37" s="19"/>
-    </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+      <c r="P36" s="18">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P37" s="18"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>246</v>
+      </c>
       <c r="B38" s="3">
         <v>1</v>
       </c>
@@ -2713,14 +2798,17 @@
         <v>161</v>
       </c>
       <c r="O38">
-        <v>99</v>
-      </c>
-      <c r="P38" s="19">
-        <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
-    </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="P38" s="18">
+        <f t="shared" si="0"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>246</v>
+      </c>
       <c r="B39" s="6">
         <v>2</v>
       </c>
@@ -2746,14 +2834,17 @@
         <v>220</v>
       </c>
       <c r="O39">
-        <v>100</v>
-      </c>
-      <c r="P39" s="19">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="P39" s="18">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>246</v>
+      </c>
       <c r="B40" s="6">
         <v>2</v>
       </c>
@@ -2779,14 +2870,17 @@
         <v>194</v>
       </c>
       <c r="O40">
-        <v>100</v>
-      </c>
-      <c r="P40" s="19">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="P40" s="18">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>246</v>
+      </c>
       <c r="B41" s="3">
         <v>2</v>
       </c>
@@ -2797,7 +2891,7 @@
         <v>193</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>227</v>
+        <v>249</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>41</v>
@@ -2812,14 +2906,17 @@
         <v>198</v>
       </c>
       <c r="O41">
-        <v>98</v>
-      </c>
-      <c r="P41" s="19">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="P41" s="18">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>246</v>
+      </c>
       <c r="B42" s="3">
         <v>4</v>
       </c>
@@ -2845,14 +2942,17 @@
         <v>186</v>
       </c>
       <c r="O42">
-        <v>498</v>
-      </c>
-      <c r="P42" s="19">
-        <f t="shared" si="0"/>
-        <v>124</v>
-      </c>
-    </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+        <v>494</v>
+      </c>
+      <c r="P42" s="18">
+        <f t="shared" si="0"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>246</v>
+      </c>
       <c r="B43" s="3">
         <v>2</v>
       </c>
@@ -2878,14 +2978,17 @@
         <v>167</v>
       </c>
       <c r="O43">
-        <v>98</v>
-      </c>
-      <c r="P43" s="19">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="P43" s="18">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>246</v>
+      </c>
       <c r="B44" s="3">
         <v>2</v>
       </c>
@@ -2911,14 +3014,17 @@
         <v>192</v>
       </c>
       <c r="O44">
-        <v>48</v>
-      </c>
-      <c r="P44" s="19">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="P44" s="18">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>246</v>
+      </c>
       <c r="B45" s="6">
         <v>3</v>
       </c>
@@ -2944,14 +3050,17 @@
         <v>226</v>
       </c>
       <c r="O45">
-        <v>500</v>
-      </c>
-      <c r="P45" s="19">
-        <f t="shared" si="0"/>
-        <v>166</v>
-      </c>
-    </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+        <v>497</v>
+      </c>
+      <c r="P45" s="18">
+        <f t="shared" si="0"/>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>246</v>
+      </c>
       <c r="B46" s="3">
         <v>2</v>
       </c>
@@ -2977,14 +3086,17 @@
         <v>170</v>
       </c>
       <c r="O46">
-        <v>98</v>
-      </c>
-      <c r="P46" s="19">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="P46" s="18">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>246</v>
+      </c>
       <c r="B47" s="3">
         <v>1</v>
       </c>
@@ -3010,14 +3122,17 @@
         <v>183</v>
       </c>
       <c r="O47">
-        <v>99</v>
-      </c>
-      <c r="P47" s="19">
-        <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
-    </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="P47" s="18">
+        <f t="shared" si="0"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>246</v>
+      </c>
       <c r="B48" s="3">
         <v>1</v>
       </c>
@@ -3043,14 +3158,17 @@
         <v>177</v>
       </c>
       <c r="O48">
-        <v>99</v>
-      </c>
-      <c r="P48" s="19">
-        <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
-    </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="P48" s="18">
+        <f t="shared" si="0"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>246</v>
+      </c>
       <c r="B49" s="3">
         <v>8</v>
       </c>
@@ -3076,14 +3194,17 @@
         <v>154</v>
       </c>
       <c r="O49">
-        <v>1000</v>
-      </c>
-      <c r="P49" s="19">
-        <f t="shared" si="0"/>
-        <v>125</v>
-      </c>
-    </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
+        <v>980</v>
+      </c>
+      <c r="P49" s="18">
+        <f t="shared" si="0"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>246</v>
+      </c>
       <c r="B50" s="6">
         <v>5</v>
       </c>
@@ -3105,14 +3226,17 @@
         <v>223</v>
       </c>
       <c r="O50">
-        <v>200</v>
-      </c>
-      <c r="P50" s="19">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+      <c r="P50" s="18">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>246</v>
+      </c>
       <c r="B51" s="3">
         <v>1</v>
       </c>
@@ -3138,14 +3262,17 @@
         <v>180</v>
       </c>
       <c r="O51">
-        <v>99</v>
-      </c>
-      <c r="P51" s="19">
-        <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
-    </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="P51" s="18">
+        <f t="shared" si="0"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>246</v>
+      </c>
       <c r="B52" s="6">
         <v>2</v>
       </c>
@@ -3171,14 +3298,17 @@
         <v>224</v>
       </c>
       <c r="O52">
-        <v>250</v>
-      </c>
-      <c r="P52" s="19">
-        <f t="shared" si="0"/>
-        <v>125</v>
-      </c>
-    </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+      <c r="P52" s="18">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>246</v>
+      </c>
       <c r="B53" s="3">
         <v>1</v>
       </c>
@@ -3204,14 +3334,17 @@
         <v>173</v>
       </c>
       <c r="O53">
-        <v>99</v>
-      </c>
-      <c r="P53" s="19">
-        <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
-    </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="P53" s="18">
+        <f t="shared" si="0"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>246</v>
+      </c>
       <c r="B54" s="3">
         <v>8</v>
       </c>
@@ -3237,17 +3370,20 @@
         <v>189</v>
       </c>
       <c r="O54">
-        <v>498</v>
-      </c>
-      <c r="P54" s="19">
-        <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
-    </row>
-    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="P55" s="19"/>
-    </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
+        <v>490</v>
+      </c>
+      <c r="P54" s="18">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P55" s="18"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>246</v>
+      </c>
       <c r="B56" s="3">
         <v>1</v>
       </c>
@@ -3273,19 +3409,19 @@
         <v>164</v>
       </c>
       <c r="O56">
-        <v>99</v>
-      </c>
-      <c r="P56" s="19">
-        <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
-    </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="P56" s="18">
+        <f t="shared" si="0"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B57" s="3">
         <v>1</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>105</v>
@@ -3314,12 +3450,15 @@
       <c r="O57">
         <v>30</v>
       </c>
-      <c r="P57" s="19">
+      <c r="P57" s="18">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>246</v>
+      </c>
       <c r="B58" s="6">
         <v>1</v>
       </c>
@@ -3344,17 +3483,20 @@
       <c r="K58" s="6"/>
       <c r="L58" s="6"/>
       <c r="M58" s="11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="O58">
-        <v>30</v>
-      </c>
-      <c r="P58" s="19">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="P58" s="18">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>246</v>
+      </c>
       <c r="B59" s="8">
         <v>1</v>
       </c>
@@ -3382,14 +3524,17 @@
         <v>33</v>
       </c>
       <c r="O59">
-        <v>28</v>
-      </c>
-      <c r="P59" s="19">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="60" spans="2:16" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="P59" s="18">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>246</v>
+      </c>
       <c r="B60" s="3">
         <v>1</v>
       </c>
@@ -3421,22 +3566,25 @@
         <v>131</v>
       </c>
       <c r="O60">
-        <v>35</v>
-      </c>
-      <c r="P60" s="19">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="P60" s="18">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>246</v>
+      </c>
       <c r="B61" s="3">
         <v>1</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>149</v>
@@ -3456,14 +3604,17 @@
         <v>151</v>
       </c>
       <c r="O61">
-        <v>29</v>
-      </c>
-      <c r="P61" s="19">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="62" spans="2:16" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="P61" s="18">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>246</v>
+      </c>
       <c r="B62" s="3">
         <v>1</v>
       </c>
@@ -3489,14 +3640,14 @@
         <v>91</v>
       </c>
       <c r="O62">
-        <v>27</v>
-      </c>
-      <c r="P62" s="19">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="63" spans="2:16" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="P62" s="18">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B63" s="3">
         <v>1</v>
       </c>
@@ -3526,12 +3677,15 @@
       <c r="O63">
         <v>29</v>
       </c>
-      <c r="P63" s="19">
+      <c r="P63" s="18">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
     </row>
-    <row r="64" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>246</v>
+      </c>
       <c r="B64" s="3">
         <v>2</v>
       </c>
@@ -3562,14 +3716,17 @@
         <v>100</v>
       </c>
       <c r="O64">
-        <v>53</v>
-      </c>
-      <c r="P64" s="19">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="65" spans="2:16" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="P64" s="18">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>246</v>
+      </c>
       <c r="B65" s="3">
         <v>1</v>
       </c>
@@ -3597,14 +3754,17 @@
         <v>136</v>
       </c>
       <c r="O65">
-        <v>29</v>
-      </c>
-      <c r="P65" s="19">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="66" spans="2:16" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="P65" s="18">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>246</v>
+      </c>
       <c r="B66" s="3">
         <v>1</v>
       </c>
@@ -3632,14 +3792,17 @@
         <v>96</v>
       </c>
       <c r="O66">
-        <v>27</v>
-      </c>
-      <c r="P66" s="19">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="67" spans="2:16" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="P66" s="18">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>246</v>
+      </c>
       <c r="B67" s="3">
         <v>1</v>
       </c>
@@ -3667,14 +3830,17 @@
         <v>29</v>
       </c>
       <c r="O67">
-        <v>27</v>
-      </c>
-      <c r="P67" s="19">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="68" spans="2:16" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="P67" s="18">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>246</v>
+      </c>
       <c r="B68" s="3">
         <v>1</v>
       </c>
@@ -3700,14 +3866,14 @@
         <v>202</v>
       </c>
       <c r="O68">
-        <v>29</v>
-      </c>
-      <c r="P68" s="19">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="69" spans="2:16" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="P68" s="18">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B69" s="3">
         <v>1</v>
       </c>
@@ -3737,27 +3903,27 @@
       <c r="O69">
         <v>29</v>
       </c>
-      <c r="P69" s="19">
+      <c r="P69" s="18">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
     </row>
-    <row r="70" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="P70" s="19"/>
-    </row>
-    <row r="71" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="P71" s="19"/>
-    </row>
-    <row r="72" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P70" s="18"/>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P71" s="18"/>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B72" s="6">
         <v>6</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D72" s="6"/>
       <c r="E72" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
@@ -3772,17 +3938,17 @@
       <c r="O72">
         <v>250</v>
       </c>
-      <c r="P72" s="19">
+      <c r="P72" s="18">
         <f t="shared" ref="P72:P73" si="1">FLOOR(O72/B72,1)</f>
         <v>41</v>
       </c>
     </row>
-    <row r="73" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B73" s="6">
         <v>1</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D73" s="6"/>
       <c r="E73" s="7"/>
@@ -3794,12 +3960,12 @@
       <c r="K73" s="6"/>
       <c r="L73" s="6"/>
       <c r="M73" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="O73">
         <v>26</v>
       </c>
-      <c r="P73" s="19">
+      <c r="P73" s="18">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Removed old files, added exported library
* Also added QR code to board; additional silkscreen indicators
</commit_message>
<xml_diff>
--- a/Eurocard-HV-piezo-driver_default_BOM_values.xlsx
+++ b/Eurocard-HV-piezo-driver_default_BOM_values.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="21075" windowHeight="10050"/>
+    <workbookView xWindow="480" yWindow="80" windowWidth="24400" windowHeight="17300"/>
   </bookViews>
   <sheets>
     <sheet name="Eurocard-HV-piezo-driver_defaul" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="246">
   <si>
     <t>Qty</t>
   </si>
@@ -670,9 +675,6 @@
     <t>D2</t>
   </si>
   <si>
-    <t>Number of kits</t>
-  </si>
-  <si>
     <t>R8, R19</t>
   </si>
   <si>
@@ -751,16 +753,7 @@
     <t>Color code</t>
   </si>
   <si>
-    <t>Quantity Available (after additional Digikey purchase)</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>NOTES</t>
-  </si>
-  <si>
-    <t>diodes need reference indicator in package!!!!!!! U6,U7 as well</t>
   </si>
   <si>
     <t>R2,R32</t>
@@ -1245,25 +1238,25 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1272,7 +1265,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1356,10 +1349,10 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1705,49 +1698,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="1"/>
     <col min="3" max="3" width="26" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="45.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="45.33203125" style="2" customWidth="1"/>
     <col min="6" max="12" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="24.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.42578125" customWidth="1"/>
+    <col min="13" max="13" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>244</v>
+    <row r="1" spans="1:16">
+      <c r="A1" s="20" t="s">
+        <v>243</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="20"/>
       <c r="B2" s="3"/>
       <c r="C2" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>247</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="19" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="B6" s="15" t="s">
         <v>0</v>
       </c>
@@ -1787,17 +1777,10 @@
       <c r="N6" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="O6" s="17" t="s">
-        <v>245</v>
-      </c>
-      <c r="P6" s="17" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>246</v>
-      </c>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+    </row>
+    <row r="7" spans="1:16" ht="28">
       <c r="B7" s="8">
         <v>20</v>
       </c>
@@ -1822,18 +1805,9 @@
       <c r="M7" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="O7">
-        <v>560</v>
-      </c>
-      <c r="P7" s="18">
-        <f>FLOOR(O7/B7,1)</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>246</v>
-      </c>
+      <c r="P7" s="18"/>
+    </row>
+    <row r="8" spans="1:16">
       <c r="B8" s="3">
         <v>1</v>
       </c>
@@ -1858,18 +1832,9 @@
       <c r="M8" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="O8">
-        <v>28</v>
-      </c>
-      <c r="P8" s="18">
-        <f t="shared" ref="P8:P69" si="0">FLOOR(O8/B8,1)</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>246</v>
-      </c>
+      <c r="P8" s="18"/>
+    </row>
+    <row r="9" spans="1:16">
       <c r="B9" s="3">
         <v>4</v>
       </c>
@@ -1894,18 +1859,9 @@
       <c r="M9" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="O9">
-        <v>112</v>
-      </c>
-      <c r="P9" s="18">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>246</v>
-      </c>
+      <c r="P9" s="18"/>
+    </row>
+    <row r="10" spans="1:16">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1930,18 +1886,9 @@
       <c r="M10" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="O10">
-        <v>28</v>
-      </c>
-      <c r="P10" s="18">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>246</v>
-      </c>
+      <c r="P10" s="18"/>
+    </row>
+    <row r="11" spans="1:16">
       <c r="B11" s="6">
         <v>1</v>
       </c>
@@ -1962,20 +1909,11 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="O11">
-        <v>99</v>
-      </c>
-      <c r="P11" s="18">
-        <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>246</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="P11" s="18"/>
+    </row>
+    <row r="12" spans="1:16" ht="42">
       <c r="B12" s="3">
         <v>27</v>
       </c>
@@ -2001,19 +1939,10 @@
         <v>44</v>
       </c>
       <c r="N12" s="3"/>
-      <c r="O12" s="5">
-        <f>973-27</f>
-        <v>946</v>
-      </c>
-      <c r="P12" s="18">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>246</v>
-      </c>
+      <c r="O12" s="5"/>
+      <c r="P12" s="18"/>
+    </row>
+    <row r="13" spans="1:16">
       <c r="B13" s="6">
         <v>1</v>
       </c>
@@ -2036,20 +1965,11 @@
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="O13">
-        <v>99</v>
-      </c>
-      <c r="P13" s="18">
-        <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>246</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="P13" s="18"/>
+    </row>
+    <row r="14" spans="1:16">
       <c r="B14" s="3">
         <v>2</v>
       </c>
@@ -2075,18 +1995,10 @@
         <v>77</v>
       </c>
       <c r="N14" s="3"/>
-      <c r="O14" s="5">
-        <v>87</v>
-      </c>
-      <c r="P14" s="18">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>246</v>
-      </c>
+      <c r="O14" s="5"/>
+      <c r="P14" s="18"/>
+    </row>
+    <row r="15" spans="1:16">
       <c r="B15" s="6">
         <v>3</v>
       </c>
@@ -2097,7 +2009,7 @@
         <v>56</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>41</v>
@@ -2111,15 +2023,9 @@
       <c r="M15" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="O15">
-        <v>97</v>
-      </c>
-      <c r="P15" s="18">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P15" s="18"/>
+    </row>
+    <row r="16" spans="1:16">
       <c r="B16" s="12">
         <v>1</v>
       </c>
@@ -2142,15 +2048,9 @@
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
       <c r="M16" s="14"/>
-      <c r="P16" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>246</v>
-      </c>
+      <c r="P16" s="18"/>
+    </row>
+    <row r="17" spans="2:16">
       <c r="B17" s="6">
         <v>1</v>
       </c>
@@ -2173,23 +2073,14 @@
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="O17">
-        <v>98</v>
-      </c>
-      <c r="P17" s="18">
-        <f t="shared" si="0"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+      <c r="P17" s="18"/>
+    </row>
+    <row r="18" spans="2:16">
       <c r="P18" s="18"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>246</v>
-      </c>
+    <row r="19" spans="2:16">
       <c r="B19" s="3">
         <v>4</v>
       </c>
@@ -2200,7 +2091,7 @@
         <v>56</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>41</v>
@@ -2215,21 +2106,13 @@
         <v>57</v>
       </c>
       <c r="N19" s="3"/>
-      <c r="O19" s="5">
-        <v>94</v>
-      </c>
-      <c r="P19" s="18">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O19" s="5"/>
+      <c r="P19" s="18"/>
+    </row>
+    <row r="20" spans="2:16">
       <c r="P20" s="18"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>246</v>
-      </c>
+    <row r="21" spans="2:16">
       <c r="B21" s="8">
         <v>1</v>
       </c>
@@ -2254,18 +2137,9 @@
       <c r="M21" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="O21">
-        <v>28</v>
-      </c>
-      <c r="P21" s="18">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>246</v>
-      </c>
+      <c r="P21" s="18"/>
+    </row>
+    <row r="22" spans="2:16">
       <c r="B22" s="3">
         <v>1</v>
       </c>
@@ -2292,18 +2166,9 @@
       <c r="M22" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="O22">
-        <v>28</v>
-      </c>
-      <c r="P22" s="18">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>246</v>
-      </c>
+      <c r="P22" s="18"/>
+    </row>
+    <row r="23" spans="2:16">
       <c r="B23" s="3">
         <v>1</v>
       </c>
@@ -2328,18 +2193,9 @@
       <c r="M23" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="O23">
-        <v>26</v>
-      </c>
-      <c r="P23" s="18">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>246</v>
-      </c>
+      <c r="P23" s="18"/>
+    </row>
+    <row r="24" spans="2:16">
       <c r="B24" s="3">
         <v>5</v>
       </c>
@@ -2366,18 +2222,9 @@
       <c r="M24" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="O24">
-        <v>140</v>
-      </c>
-      <c r="P24" s="18">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>246</v>
-      </c>
+      <c r="P24" s="18"/>
+    </row>
+    <row r="25" spans="2:16">
       <c r="B25" s="3">
         <v>1</v>
       </c>
@@ -2402,15 +2249,9 @@
       <c r="M25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O25">
-        <v>26</v>
-      </c>
-      <c r="P25" s="18">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P25" s="18"/>
+    </row>
+    <row r="26" spans="2:16">
       <c r="B26" s="3">
         <v>2</v>
       </c>
@@ -2435,15 +2276,9 @@
       <c r="M26" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="O26">
-        <v>50</v>
-      </c>
-      <c r="P26" s="18">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P26" s="18"/>
+    </row>
+    <row r="27" spans="2:16">
       <c r="B27" s="1">
         <v>3</v>
       </c>
@@ -2468,23 +2303,17 @@
       <c r="M27" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="P27" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>246</v>
-      </c>
+      <c r="P27" s="18"/>
+    </row>
+    <row r="28" spans="2:16">
       <c r="B28" s="6">
         <v>1</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>111</v>
@@ -2507,20 +2336,11 @@
         <v>115</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="O28">
-        <v>29</v>
-      </c>
-      <c r="P28" s="18">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>246</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="P28" s="18"/>
+    </row>
+    <row r="29" spans="2:16">
       <c r="B29" s="3">
         <v>1</v>
       </c>
@@ -2547,15 +2367,9 @@
       <c r="M29" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="O29">
-        <v>29</v>
-      </c>
-      <c r="P29" s="18">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P29" s="18"/>
+    </row>
+    <row r="30" spans="2:16">
       <c r="B30" s="1">
         <v>1</v>
       </c>
@@ -2574,12 +2388,9 @@
       <c r="M30" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="P30" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P30" s="18"/>
+    </row>
+    <row r="31" spans="2:16">
       <c r="B31" s="6">
         <v>2</v>
       </c>
@@ -2606,15 +2417,9 @@
       <c r="M31" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="O31">
-        <v>100</v>
-      </c>
-      <c r="P31" s="18">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P31" s="18"/>
+    </row>
+    <row r="32" spans="2:16">
       <c r="B32" s="6">
         <v>1</v>
       </c>
@@ -2641,15 +2446,9 @@
       <c r="M32" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="O32">
-        <v>50</v>
-      </c>
-      <c r="P32" s="18">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P32" s="18"/>
+    </row>
+    <row r="33" spans="2:16">
       <c r="B33" s="6">
         <v>1</v>
       </c>
@@ -2674,15 +2473,9 @@
       <c r="M33" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="O33">
-        <v>29</v>
-      </c>
-      <c r="P33" s="18">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P33" s="18"/>
+    </row>
+    <row r="34" spans="2:16">
       <c r="B34" s="1">
         <v>1</v>
       </c>
@@ -2701,12 +2494,9 @@
       <c r="M34" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="P34" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P34" s="18"/>
+    </row>
+    <row r="35" spans="2:16">
       <c r="B35" s="1">
         <v>1</v>
       </c>
@@ -2725,15 +2515,9 @@
       <c r="G35" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="P35" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>246</v>
-      </c>
+      <c r="P35" s="18"/>
+    </row>
+    <row r="36" spans="2:16">
       <c r="B36" s="3">
         <v>10</v>
       </c>
@@ -2758,21 +2542,12 @@
       <c r="M36" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="O36">
-        <v>280</v>
-      </c>
-      <c r="P36" s="18">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P36" s="18"/>
+    </row>
+    <row r="37" spans="2:16">
       <c r="P37" s="18"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>246</v>
-      </c>
+    <row r="38" spans="2:16">
       <c r="B38" s="3">
         <v>1</v>
       </c>
@@ -2797,18 +2572,9 @@
       <c r="M38" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="O38">
-        <v>98</v>
-      </c>
-      <c r="P38" s="18">
-        <f t="shared" si="0"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>246</v>
-      </c>
+      <c r="P38" s="18"/>
+    </row>
+    <row r="39" spans="2:16">
       <c r="B39" s="6">
         <v>2</v>
       </c>
@@ -2819,7 +2585,7 @@
         <v>193</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>41</v>
@@ -2831,20 +2597,11 @@
       <c r="K39" s="6"/>
       <c r="L39" s="6"/>
       <c r="M39" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="O39">
-        <v>98</v>
-      </c>
-      <c r="P39" s="18">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>246</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="P39" s="18"/>
+    </row>
+    <row r="40" spans="2:16">
       <c r="B40" s="6">
         <v>2</v>
       </c>
@@ -2855,7 +2612,7 @@
         <v>193</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>41</v>
@@ -2869,18 +2626,9 @@
       <c r="M40" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="O40">
-        <v>98</v>
-      </c>
-      <c r="P40" s="18">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>246</v>
-      </c>
+      <c r="P40" s="18"/>
+    </row>
+    <row r="41" spans="2:16">
       <c r="B41" s="3">
         <v>2</v>
       </c>
@@ -2891,7 +2639,7 @@
         <v>193</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>41</v>
@@ -2905,18 +2653,9 @@
       <c r="M41" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="O41">
-        <v>95</v>
-      </c>
-      <c r="P41" s="18">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>246</v>
-      </c>
+      <c r="P41" s="18"/>
+    </row>
+    <row r="42" spans="2:16">
       <c r="B42" s="3">
         <v>4</v>
       </c>
@@ -2941,18 +2680,9 @@
       <c r="M42" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="O42">
-        <v>494</v>
-      </c>
-      <c r="P42" s="18">
-        <f t="shared" si="0"/>
-        <v>123</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>246</v>
-      </c>
+      <c r="P42" s="18"/>
+    </row>
+    <row r="43" spans="2:16">
       <c r="B43" s="3">
         <v>2</v>
       </c>
@@ -2977,18 +2707,9 @@
       <c r="M43" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="O43">
-        <v>96</v>
-      </c>
-      <c r="P43" s="18">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>246</v>
-      </c>
+      <c r="P43" s="18"/>
+    </row>
+    <row r="44" spans="2:16">
       <c r="B44" s="3">
         <v>2</v>
       </c>
@@ -3013,18 +2734,9 @@
       <c r="M44" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="O44">
-        <v>46</v>
-      </c>
-      <c r="P44" s="18">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>246</v>
-      </c>
+      <c r="P44" s="18"/>
+    </row>
+    <row r="45" spans="2:16">
       <c r="B45" s="6">
         <v>3</v>
       </c>
@@ -3047,20 +2759,11 @@
       <c r="K45" s="6"/>
       <c r="L45" s="6"/>
       <c r="M45" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="O45">
-        <v>497</v>
-      </c>
-      <c r="P45" s="18">
-        <f t="shared" si="0"/>
-        <v>165</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>246</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="P45" s="18"/>
+    </row>
+    <row r="46" spans="2:16">
       <c r="B46" s="3">
         <v>2</v>
       </c>
@@ -3085,18 +2788,9 @@
       <c r="M46" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="O46">
-        <v>96</v>
-      </c>
-      <c r="P46" s="18">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>246</v>
-      </c>
+      <c r="P46" s="18"/>
+    </row>
+    <row r="47" spans="2:16">
       <c r="B47" s="3">
         <v>1</v>
       </c>
@@ -3121,18 +2815,9 @@
       <c r="M47" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="O47">
-        <v>98</v>
-      </c>
-      <c r="P47" s="18">
-        <f t="shared" si="0"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>246</v>
-      </c>
+      <c r="P47" s="18"/>
+    </row>
+    <row r="48" spans="2:16">
       <c r="B48" s="3">
         <v>1</v>
       </c>
@@ -3157,18 +2842,9 @@
       <c r="M48" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="O48">
-        <v>98</v>
-      </c>
-      <c r="P48" s="18">
-        <f t="shared" si="0"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>246</v>
-      </c>
+      <c r="P48" s="18"/>
+    </row>
+    <row r="49" spans="2:16">
       <c r="B49" s="3">
         <v>8</v>
       </c>
@@ -3179,7 +2855,7 @@
         <v>153</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>41</v>
@@ -3193,18 +2869,9 @@
       <c r="M49" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="O49">
-        <v>980</v>
-      </c>
-      <c r="P49" s="18">
-        <f t="shared" si="0"/>
-        <v>122</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>246</v>
-      </c>
+      <c r="P49" s="18"/>
+    </row>
+    <row r="50" spans="2:16">
       <c r="B50" s="6">
         <v>5</v>
       </c>
@@ -3213,7 +2880,7 @@
       </c>
       <c r="D50" s="6"/>
       <c r="E50" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
@@ -3223,20 +2890,11 @@
       <c r="K50" s="6"/>
       <c r="L50" s="6"/>
       <c r="M50" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="O50">
-        <v>195</v>
-      </c>
-      <c r="P50" s="18">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>246</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="P50" s="18"/>
+    </row>
+    <row r="51" spans="2:16">
       <c r="B51" s="3">
         <v>1</v>
       </c>
@@ -3261,18 +2919,9 @@
       <c r="M51" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="O51">
-        <v>98</v>
-      </c>
-      <c r="P51" s="18">
-        <f t="shared" si="0"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>246</v>
-      </c>
+      <c r="P51" s="18"/>
+    </row>
+    <row r="52" spans="2:16">
       <c r="B52" s="6">
         <v>2</v>
       </c>
@@ -3295,20 +2944,11 @@
       <c r="K52" s="6"/>
       <c r="L52" s="6"/>
       <c r="M52" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="O52">
-        <v>248</v>
-      </c>
-      <c r="P52" s="18">
-        <f t="shared" si="0"/>
-        <v>124</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>246</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="P52" s="18"/>
+    </row>
+    <row r="53" spans="2:16">
       <c r="B53" s="3">
         <v>1</v>
       </c>
@@ -3333,18 +2973,9 @@
       <c r="M53" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="O53">
-        <v>98</v>
-      </c>
-      <c r="P53" s="18">
-        <f t="shared" si="0"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>246</v>
-      </c>
+      <c r="P53" s="18"/>
+    </row>
+    <row r="54" spans="2:16">
       <c r="B54" s="3">
         <v>8</v>
       </c>
@@ -3369,21 +3000,12 @@
       <c r="M54" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="O54">
-        <v>490</v>
-      </c>
-      <c r="P54" s="18">
-        <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P54" s="18"/>
+    </row>
+    <row r="55" spans="2:16">
       <c r="P55" s="18"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>246</v>
-      </c>
+    <row r="56" spans="2:16">
       <c r="B56" s="3">
         <v>1</v>
       </c>
@@ -3408,20 +3030,14 @@
       <c r="M56" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="O56">
-        <v>98</v>
-      </c>
-      <c r="P56" s="18">
-        <f t="shared" si="0"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P56" s="18"/>
+    </row>
+    <row r="57" spans="2:16">
       <c r="B57" s="3">
         <v>1</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>105</v>
@@ -3447,18 +3063,9 @@
       <c r="M57" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="O57">
-        <v>30</v>
-      </c>
-      <c r="P57" s="18">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>246</v>
-      </c>
+      <c r="P57" s="18"/>
+    </row>
+    <row r="58" spans="2:16">
       <c r="B58" s="6">
         <v>1</v>
       </c>
@@ -3483,20 +3090,11 @@
       <c r="K58" s="6"/>
       <c r="L58" s="6"/>
       <c r="M58" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="O58">
-        <v>29</v>
-      </c>
-      <c r="P58" s="18">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>246</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="P58" s="18"/>
+    </row>
+    <row r="59" spans="2:16">
       <c r="B59" s="8">
         <v>1</v>
       </c>
@@ -3523,18 +3121,9 @@
       <c r="M59" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="O59">
-        <v>27</v>
-      </c>
-      <c r="P59" s="18">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>246</v>
-      </c>
+      <c r="P59" s="18"/>
+    </row>
+    <row r="60" spans="2:16">
       <c r="B60" s="3">
         <v>1</v>
       </c>
@@ -3565,26 +3154,17 @@
       <c r="M60" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="O60">
-        <v>33</v>
-      </c>
-      <c r="P60" s="18">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>246</v>
-      </c>
+      <c r="P60" s="18"/>
+    </row>
+    <row r="61" spans="2:16">
       <c r="B61" s="3">
         <v>1</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>149</v>
@@ -3603,18 +3183,9 @@
       <c r="M61" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="O61">
-        <v>28</v>
-      </c>
-      <c r="P61" s="18">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>246</v>
-      </c>
+      <c r="P61" s="18"/>
+    </row>
+    <row r="62" spans="2:16">
       <c r="B62" s="3">
         <v>1</v>
       </c>
@@ -3639,15 +3210,9 @@
       <c r="M62" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="O62">
-        <v>26</v>
-      </c>
-      <c r="P62" s="18">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P62" s="18"/>
+    </row>
+    <row r="63" spans="2:16">
       <c r="B63" s="3">
         <v>1</v>
       </c>
@@ -3674,18 +3239,9 @@
       <c r="M63" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="O63">
-        <v>29</v>
-      </c>
-      <c r="P63" s="18">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>246</v>
-      </c>
+      <c r="P63" s="18"/>
+    </row>
+    <row r="64" spans="2:16">
       <c r="B64" s="3">
         <v>2</v>
       </c>
@@ -3715,18 +3271,9 @@
       <c r="N64" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="O64">
-        <v>51</v>
-      </c>
-      <c r="P64" s="18">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>246</v>
-      </c>
+      <c r="P64" s="18"/>
+    </row>
+    <row r="65" spans="2:16">
       <c r="B65" s="3">
         <v>1</v>
       </c>
@@ -3753,18 +3300,9 @@
       <c r="M65" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="O65">
-        <v>28</v>
-      </c>
-      <c r="P65" s="18">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>246</v>
-      </c>
+      <c r="P65" s="18"/>
+    </row>
+    <row r="66" spans="2:16">
       <c r="B66" s="3">
         <v>1</v>
       </c>
@@ -3791,18 +3329,9 @@
       <c r="M66" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="O66">
-        <v>26</v>
-      </c>
-      <c r="P66" s="18">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>246</v>
-      </c>
+      <c r="P66" s="18"/>
+    </row>
+    <row r="67" spans="2:16">
       <c r="B67" s="3">
         <v>1</v>
       </c>
@@ -3829,18 +3358,9 @@
       <c r="M67" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="O67">
-        <v>26</v>
-      </c>
-      <c r="P67" s="18">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>246</v>
-      </c>
+      <c r="P67" s="18"/>
+    </row>
+    <row r="68" spans="2:16">
       <c r="B68" s="3">
         <v>1</v>
       </c>
@@ -3865,15 +3385,9 @@
       <c r="M68" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="O68">
-        <v>28</v>
-      </c>
-      <c r="P68" s="18">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P68" s="18"/>
+    </row>
+    <row r="69" spans="2:16">
       <c r="B69" s="3">
         <v>1</v>
       </c>
@@ -3900,30 +3414,24 @@
       <c r="M69" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="O69">
-        <v>29</v>
-      </c>
-      <c r="P69" s="18">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P69" s="18"/>
+    </row>
+    <row r="70" spans="2:16">
       <c r="P70" s="18"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:16">
       <c r="P71" s="18"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:16">
       <c r="B72" s="6">
         <v>6</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D72" s="6"/>
       <c r="E72" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
@@ -3935,20 +3443,14 @@
       <c r="M72" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="O72">
-        <v>250</v>
-      </c>
-      <c r="P72" s="18">
-        <f t="shared" ref="P72:P73" si="1">FLOOR(O72/B72,1)</f>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P72" s="18"/>
+    </row>
+    <row r="73" spans="2:16">
       <c r="B73" s="6">
         <v>1</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D73" s="6"/>
       <c r="E73" s="7"/>
@@ -3960,15 +3462,9 @@
       <c r="K73" s="6"/>
       <c r="L73" s="6"/>
       <c r="M73" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="O73">
-        <v>26</v>
-      </c>
-      <c r="P73" s="18">
-        <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="P73" s="18"/>
     </row>
   </sheetData>
   <sortState ref="B2:N65">
@@ -3981,6 +3477,10 @@
     <hyperlink ref="M58" r:id="rId1" display="http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=194050138&amp;uq=635956463589417549"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>